<commit_message>
adding and fixing translations
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
+++ b/odkx/app/config/tables/fw_location/forms/fw_location/fw_location.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -164,7 +164,10 @@
     <t xml:space="preserve">The household id is {{data.hh_id}}</t>
   </si>
   <si>
-    <t xml:space="preserve">HHID: {{data.hh_id}}</t>
+    <t xml:space="preserve">Identificação do agregado{{data.hh_id}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utambulisho wa Kaya {{data.hh_id}}</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -258,6 +261,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -361,7 +368,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -406,10 +413,10 @@
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.49"/>
@@ -472,10 +479,10 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.37"/>
@@ -612,7 +619,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.67578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -676,10 +683,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
@@ -713,22 +720,22 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>46</v>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:D1048576">
+  <conditionalFormatting sqref="B1:B1048576 C1:D2 C4:D1048576">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>

</xml_diff>